<commit_message>
looking for all words
</commit_message>
<xml_diff>
--- a/spreadSheets/known.xlsx
+++ b/spreadSheets/known.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doosan-my.sharepoint.com/personal/milanhutera_corp_doosan_com/Documents/Python/subtitles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doosan-my.sharepoint.com/personal/milanhutera_corp_doosan_com/Documents/Python/subtitles/spreadSheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{FAC50869-412F-4697-9323-4A76DFCD199C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C90C07E7-890A-4067-A67B-6C7EB7D6CE59}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{FAC50869-412F-4697-9323-4A76DFCD199C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DCF67894-3937-46D3-A588-A0EA7436E823}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CZ_words" sheetId="1" r:id="rId1"/>
@@ -5319,16 +5319,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" activeCellId="2" sqref="A1:A1048576 C1:C1048576 D1:D1048576"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5341,8 +5341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A1657"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1582" workbookViewId="0">
-      <selection activeCell="A1593" sqref="A1593:XFD1593"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1623" sqref="A1623"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>